<commit_message>
Edit table Staff in excel file
</commit_message>
<xml_diff>
--- a/Document/Design Entities In More Detail.xlsx
+++ b/Document/Design Entities In More Detail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Internship Book Store Management\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-Book-Store-Management-Project\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FDB43F-59ED-4AA1-ADF9-24BE8CA44322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CA6659-4A97-4896-8BE9-46E57E98E769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="10" xr2:uid="{7A4C3B00-C6B5-404D-B167-C76F43FDFE12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{7A4C3B00-C6B5-404D-B167-C76F43FDFE12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sach" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -288,9 +287,6 @@
     <t>Số́ FAX</t>
   </si>
   <si>
-    <t>NVachHang</t>
-  </si>
-  <si>
     <t>tenNV</t>
   </si>
   <si>
@@ -361,6 +357,9 @@
   </si>
   <si>
     <t>Giá bán</t>
+  </si>
+  <si>
+    <t>NhanVien</t>
   </si>
 </sst>
 </file>
@@ -535,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -546,7 +545,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -897,13 +895,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1024,7 +1022,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
@@ -1034,12 +1032,12 @@
         <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
@@ -1049,7 +1047,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1064,7 +1062,7 @@
         <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1095,13 +1093,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="16"/>
+      <c r="A1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1122,7 +1120,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1134,12 +1132,12 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -1151,16 +1149,16 @@
         <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1168,7 +1166,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1183,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A98589-4768-4C99-BF9E-4DEC7D5F3EB0}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -1198,13 +1196,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="A1" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1224,8 +1222,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>101</v>
+      <c r="A3" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>11</v>
@@ -1234,15 +1232,15 @@
         <v>16</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>96</v>
+      <c r="A4" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>11</v>
@@ -1254,11 +1252,11 @@
         <v>17</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -1275,8 +1273,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>88</v>
+      <c r="A6" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>9</v>
@@ -1288,7 +1286,7 @@
         <v>36</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1303,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4027414-FDDC-40F6-9BFF-5DD594764020}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,13 +1316,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="A1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1362,7 +1360,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -1374,12 +1372,12 @@
         <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>42</v>
@@ -1389,7 +1387,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,7 +1436,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1454,7 +1452,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,13 +1465,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1587,13 +1585,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1690,10 +1688,10 @@
       <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1724,13 +1722,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1856,7 +1854,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,13 +1868,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -2021,7 +2019,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,13 +2033,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -2134,10 +2132,10 @@
         <v>43</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2149,10 +2147,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2169,7 +2167,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,13 +2181,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2284,13 +2282,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">

</xml_diff>